<commit_message>
Course list ETL engine
</commit_message>
<xml_diff>
--- a/content/Videos.xlsx
+++ b/content/Videos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\hau-ai-powered-lms\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hau-ai-powered-lms\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFA04FC-20D6-4008-98FE-BB42070D6202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935400C-15C1-4283-B68B-A418FE68072B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="210" windowWidth="10875" windowHeight="9840" xr2:uid="{5ECA9A81-29B9-4D96-8F46-91117AAAFF35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECA9A81-29B9-4D96-8F46-91117AAAFF35}"/>
   </bookViews>
   <sheets>
     <sheet name="MVP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>AWS Machine Learning University</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve">In this video, we go over the course overview, learning outcomes and machine learning resources that we will use in this class. </t>
+  </si>
+  <si>
+    <t>Natural Language Processing (NLP)</t>
   </si>
 </sst>
 </file>
@@ -670,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC9C4D9-2C16-4CAB-BF03-0C5497B266BE}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
         <v>88</v>

</xml_diff>